<commit_message>
438: necessario valorizzare le seguenti colonne:S
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap 3.0
subject_application_version: 20.17.02
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20241227/Winsap_3.0/20.17.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{495F3AB5-F33E-4185-90F6-66EB6A8D03B1}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29C0E34C-7E7F-46C0-9601-32366DBEF55C}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-4740" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1823,9 +1823,6 @@
     <t>2.16.840.1.113883.2.9.2.150907.e87afe51e8ba20fc26491f59439a800e61556f8af6154c9d9b6a9b101cb5ec3c.a6338b22ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>[ERRORE-b195| Sezione Diagnosi: L'elemento entry/organizer/component/observation (Linfonodi) deve avere l'elemento value con @xsi:type='IVL_PQ', che identifica il numero dei linfonodi.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAP_CT20_KO</t>
   </si>
   <si>
@@ -2033,6 +2030,9 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>[ERRORE-b195| Sezione Diagnosi: L'elemento entry/organizer/component/observation (Linfonodi) deve avere l'elemento value con @xsi:type='IVL_PQ', che identifica il numero dei linfonodi.]</t>
   </si>
 </sst>
 </file>
@@ -4475,10 +4475,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="H198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A209" sqref="A209"/>
+      <selection pane="bottomRight" activeCell="O211" sqref="O211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12347,7 +12347,7 @@
         <v>120</v>
       </c>
       <c r="O210" s="66" t="s">
-        <v>465</v>
+        <v>531</v>
       </c>
       <c r="P210" s="66" t="s">
         <v>120</v>
@@ -12379,22 +12379,22 @@
         <v>414</v>
       </c>
       <c r="D211" s="51" t="s">
+        <v>465</v>
+      </c>
+      <c r="E211" s="59" t="s">
         <v>466</v>
-      </c>
-      <c r="E211" s="59" t="s">
-        <v>467</v>
       </c>
       <c r="F211" s="64">
         <v>45631</v>
       </c>
       <c r="G211" s="65" t="s">
+        <v>467</v>
+      </c>
+      <c r="H211" s="65" t="s">
         <v>468</v>
       </c>
-      <c r="H211" s="65" t="s">
+      <c r="I211" s="65" t="s">
         <v>469</v>
-      </c>
-      <c r="I211" s="65" t="s">
-        <v>470</v>
       </c>
       <c r="J211" s="66" t="s">
         <v>120</v>
@@ -12408,7 +12408,7 @@
         <v>120</v>
       </c>
       <c r="O211" s="66" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P211" s="66" t="s">
         <v>120</v>
@@ -12440,22 +12440,22 @@
         <v>414</v>
       </c>
       <c r="D212" s="51" t="s">
+        <v>471</v>
+      </c>
+      <c r="E212" s="59" t="s">
         <v>472</v>
-      </c>
-      <c r="E212" s="59" t="s">
-        <v>473</v>
       </c>
       <c r="F212" s="53">
         <v>45631</v>
       </c>
       <c r="G212" s="54" t="s">
+        <v>473</v>
+      </c>
+      <c r="H212" s="54" t="s">
         <v>474</v>
       </c>
-      <c r="H212" s="54" t="s">
+      <c r="I212" s="54" t="s">
         <v>475</v>
-      </c>
-      <c r="I212" s="54" t="s">
-        <v>476</v>
       </c>
       <c r="J212" s="55" t="s">
         <v>120</v>
@@ -12469,7 +12469,7 @@
         <v>120</v>
       </c>
       <c r="O212" s="55" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="P212" s="55" t="s">
         <v>120</v>
@@ -12501,22 +12501,22 @@
         <v>414</v>
       </c>
       <c r="D213" s="41" t="s">
+        <v>477</v>
+      </c>
+      <c r="E213" s="42" t="s">
         <v>478</v>
-      </c>
-      <c r="E213" s="42" t="s">
-        <v>479</v>
       </c>
       <c r="F213" s="64">
         <v>45631</v>
       </c>
       <c r="G213" s="79" t="s">
+        <v>479</v>
+      </c>
+      <c r="H213" s="79" t="s">
         <v>480</v>
       </c>
-      <c r="H213" s="79" t="s">
+      <c r="I213" s="80" t="s">
         <v>481</v>
-      </c>
-      <c r="I213" s="80" t="s">
-        <v>482</v>
       </c>
       <c r="J213" s="81" t="s">
         <v>120</v>
@@ -12530,7 +12530,7 @@
         <v>120</v>
       </c>
       <c r="O213" s="73" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="P213" s="81" t="s">
         <v>120</v>
@@ -12562,10 +12562,10 @@
         <v>414</v>
       </c>
       <c r="D214" s="50" t="s">
+        <v>483</v>
+      </c>
+      <c r="E214" s="52" t="s">
         <v>484</v>
-      </c>
-      <c r="E214" s="52" t="s">
-        <v>485</v>
       </c>
       <c r="F214" s="64"/>
       <c r="G214" s="65"/>
@@ -12603,10 +12603,10 @@
         <v>100</v>
       </c>
       <c r="D215" s="50" t="s">
+        <v>485</v>
+      </c>
+      <c r="E215" s="52" t="s">
         <v>486</v>
-      </c>
-      <c r="E215" s="52" t="s">
-        <v>487</v>
       </c>
       <c r="F215" s="53"/>
       <c r="G215" s="54"/>
@@ -12640,10 +12640,10 @@
         <v>100</v>
       </c>
       <c r="D216" s="50" t="s">
+        <v>487</v>
+      </c>
+      <c r="E216" s="52" t="s">
         <v>488</v>
-      </c>
-      <c r="E216" s="52" t="s">
-        <v>489</v>
       </c>
       <c r="F216" s="53"/>
       <c r="G216" s="54"/>
@@ -12677,10 +12677,10 @@
         <v>102</v>
       </c>
       <c r="D217" s="41" t="s">
+        <v>489</v>
+      </c>
+      <c r="E217" s="42" t="s">
         <v>490</v>
-      </c>
-      <c r="E217" s="42" t="s">
-        <v>491</v>
       </c>
       <c r="F217" s="43"/>
       <c r="G217" s="44"/>
@@ -12714,10 +12714,10 @@
         <v>102</v>
       </c>
       <c r="D218" s="50" t="s">
+        <v>491</v>
+      </c>
+      <c r="E218" s="52" t="s">
         <v>492</v>
-      </c>
-      <c r="E218" s="52" t="s">
-        <v>493</v>
       </c>
       <c r="F218" s="53"/>
       <c r="G218" s="54"/>
@@ -12751,22 +12751,22 @@
         <v>414</v>
       </c>
       <c r="D219" s="50" t="s">
+        <v>493</v>
+      </c>
+      <c r="E219" s="52" t="s">
         <v>494</v>
-      </c>
-      <c r="E219" s="52" t="s">
-        <v>495</v>
       </c>
       <c r="F219" s="53">
         <v>45653</v>
       </c>
       <c r="G219" s="54" t="s">
+        <v>495</v>
+      </c>
+      <c r="H219" s="54" t="s">
         <v>496</v>
       </c>
-      <c r="H219" s="54" t="s">
+      <c r="I219" s="54" t="s">
         <v>497</v>
-      </c>
-      <c r="I219" s="54" t="s">
-        <v>498</v>
       </c>
       <c r="J219" s="55" t="s">
         <v>120</v>
@@ -16958,12 +16958,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -16978,12 +16978,12 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -16993,7 +16993,7 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
   </sheetData>
@@ -17023,22 +17023,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>505</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="15" t="s">
         <v>506</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>507</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17046,13 +17046,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>509</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>510</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17060,13 +17060,13 @@
         <v>60</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>512</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17074,13 +17074,13 @@
         <v>102</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C4" s="12">
         <v>446.447</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17088,13 +17088,13 @@
         <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>515</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17102,13 +17102,13 @@
         <v>78</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>517</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -17116,13 +17116,13 @@
         <v>87</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>519</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -17130,13 +17130,13 @@
         <v>104</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>521</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -17144,27 +17144,27 @@
         <v>100</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>522</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>523</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>526</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17172,13 +17172,13 @@
         <v>414</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>527</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>528</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18160,7 +18160,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>120</v>
@@ -18168,7 +18168,7 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>431</v>
@@ -19185,6 +19185,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A6B8B41AB45FE4E8B23889C5F604192" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="c6632d705a2655bc4ef003303aa3e89d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="228e3216-9b37-47f7-9d85-6e6726edc181" xmlns:ns3="1e0ec522-3181-4f7c-b363-2ace71f6fee9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc3f6e4344a62cf01cb5a4907fa5259c" ns2:_="" ns3:_="">
     <xsd:import namespace="228e3216-9b37-47f7-9d85-6e6726edc181"/>
@@ -19379,27 +19399,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
+    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E288F5C3-DA90-4167-B23D-BE3846B1C7D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19416,23 +19435,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
-    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Accreditamento Winsap 3.0 Anatomia Patologica #4.1
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap 3.0
subject_application_version: 20.17.02
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20241227/Winsap_3.0/20.17.02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20250204/Winsap_3.0/20.17.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29C0E34C-7E7F-46C0-9601-32366DBEF55C}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C52122AD-8EC9-4514-ABFD-29C92C06ADC6}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4740" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1667,15 +1667,6 @@
 Il Documento CDA2 Anatomia Patologica dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-12-05T10:53:12Z</t>
-  </si>
-  <si>
-    <t>5d94766d63a773e6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.a52a8103fe8a8464dba5fa9a95b3c61eee263ea600925bc69290c16f0f8e91a2.3540bd52f6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAP_CT2</t>
   </si>
   <si>
@@ -1684,15 +1675,6 @@
 </t>
   </si>
   <si>
-    <t>2024-12-05T15:51:13Z</t>
-  </si>
-  <si>
-    <t>0de42c47914151e2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.5219a9943372e960a87a0722fa3a5e2e9cecfed7ad94360d514dbbb901e56380.4d4055e69c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAP_CT3</t>
   </si>
   <si>
@@ -1701,15 +1683,6 @@
 </t>
   </si>
   <si>
-    <t>2024-12-09T11:14:06Z</t>
-  </si>
-  <si>
-    <t>f82172c63b7651c2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.f3ff60d6fa522f6dff88da2d32805212986143f217de1948a75c4b4cf7f8c51d.4773bff354^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_TOKEN_JWT_RAP_KO</t>
   </si>
   <si>
@@ -1821,6 +1794,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150907.e87afe51e8ba20fc26491f59439a800e61556f8af6154c9d9b6a9b101cb5ec3c.a6338b22ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>[ERRORE-b195| Sezione Diagnosi: L'elemento entry/organizer/component/observation (Linfonodi) deve avere l'elemento value con @xsi:type='IVL_PQ', che identifica il numero dei linfonodi.]</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAP_CT20_KO</t>
@@ -1924,15 +1900,6 @@
 Il Documento CDA2 Anatomia Patologica dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RAP" e "CDA2_Referto_di_Anatomia_Patologica_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2024-12-27T11:29:05Z</t>
-  </si>
-  <si>
-    <t>6ddb6b37a69748db</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.ddded146e02c8b8874a9b394f634adc908b35e3c30b9f26ff92fe50c76e6e0b8.90f5c31e66^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Razionale di Applicabilità</t>
   </si>
   <si>
@@ -2032,7 +1999,40 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>[ERRORE-b195| Sezione Diagnosi: L'elemento entry/organizer/component/observation (Linfonodi) deve avere l'elemento value con @xsi:type='IVL_PQ', che identifica il numero dei linfonodi.]</t>
+    <t>26004ddeb65cdb05</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.ad2187981e3f1491e0f61bad9cb38712eb68570f21a458e6abe68e0ab261a64e.82a4f3fcf0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T10:48:18Z</t>
+  </si>
+  <si>
+    <t>2025-02-04T10:55:44Z</t>
+  </si>
+  <si>
+    <t>440e503517887dcb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.a71a4388c14664fc26e635f3b616a6eab07d795b701d9f97963470a3b5a3c7ff.e0bb7c4853^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T11:04:41Z</t>
+  </si>
+  <si>
+    <t>c15ec2de72bcc112</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.ad0f64eda4cf289190ce3ee1bbdadbf02a18a5888deb3e86d332b19eb5888a64.bf21883adb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T11:28:20Z</t>
+  </si>
+  <si>
+    <t>d30936b556cc1dd7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.64cf9f7b3941664ec24b7147a6910f9b066d7399aa26950f34b98bb71ccc1651.867a8914a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4475,10 +4475,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O211" sqref="O211"/>
+      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11754,16 +11754,16 @@
         <v>416</v>
       </c>
       <c r="F198" s="64">
-        <v>45631</v>
+        <v>45692</v>
       </c>
       <c r="G198" s="65" t="s">
-        <v>417</v>
+        <v>522</v>
       </c>
       <c r="H198" s="65" t="s">
-        <v>418</v>
+        <v>520</v>
       </c>
       <c r="I198" s="65" t="s">
-        <v>419</v>
+        <v>521</v>
       </c>
       <c r="J198" s="66" t="s">
         <v>120</v>
@@ -11795,22 +11795,22 @@
         <v>414</v>
       </c>
       <c r="D199" s="51" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E199" s="59" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="F199" s="64">
-        <v>45631</v>
+        <v>45692</v>
       </c>
       <c r="G199" s="65" t="s">
-        <v>422</v>
+        <v>523</v>
       </c>
       <c r="H199" s="65" t="s">
-        <v>423</v>
+        <v>524</v>
       </c>
       <c r="I199" s="65" t="s">
-        <v>424</v>
+        <v>525</v>
       </c>
       <c r="J199" s="66" t="s">
         <v>120</v>
@@ -11842,22 +11842,22 @@
         <v>414</v>
       </c>
       <c r="D200" s="51" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="E200" s="59" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="F200" s="64">
-        <v>45635</v>
+        <v>45692</v>
       </c>
       <c r="G200" s="65" t="s">
-        <v>427</v>
+        <v>529</v>
       </c>
       <c r="H200" s="65" t="s">
-        <v>428</v>
+        <v>530</v>
       </c>
       <c r="I200" s="65" t="s">
-        <v>429</v>
+        <v>531</v>
       </c>
       <c r="J200" s="66" t="s">
         <v>120</v>
@@ -11889,7 +11889,7 @@
         <v>414</v>
       </c>
       <c r="D201" s="51" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="E201" s="59" t="s">
         <v>97</v>
@@ -11899,10 +11899,10 @@
       <c r="H201" s="71"/>
       <c r="I201" s="71"/>
       <c r="J201" s="72" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K201" s="72" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="L201" s="72"/>
       <c r="M201" s="72" t="s">
@@ -11934,7 +11934,7 @@
         <v>414</v>
       </c>
       <c r="D202" s="51" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="E202" s="59" t="s">
         <v>110</v>
@@ -11944,10 +11944,10 @@
       <c r="H202" s="71"/>
       <c r="I202" s="71"/>
       <c r="J202" s="72" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K202" s="72" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="L202" s="72"/>
       <c r="M202" s="72" t="s">
@@ -11979,10 +11979,10 @@
         <v>414</v>
       </c>
       <c r="D203" s="51" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="E203" s="59" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="F203" s="64">
         <v>45631</v>
@@ -11996,10 +11996,10 @@
       <c r="K203" s="72"/>
       <c r="L203" s="72"/>
       <c r="M203" s="72" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="N203" s="72" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="O203" s="72"/>
       <c r="P203" s="72" t="s">
@@ -12009,10 +12009,10 @@
         <v>120</v>
       </c>
       <c r="R203" s="72" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="S203" s="72" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="T203" s="72"/>
       <c r="U203" s="74"/>
@@ -12032,20 +12032,20 @@
         <v>414</v>
       </c>
       <c r="D204" s="51" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="E204" s="59" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="F204" s="64"/>
       <c r="G204" s="65"/>
       <c r="H204" s="65"/>
       <c r="I204" s="65"/>
       <c r="J204" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K204" s="66" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="L204" s="66"/>
       <c r="M204" s="66"/>
@@ -12073,20 +12073,20 @@
         <v>414</v>
       </c>
       <c r="D205" s="51" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="E205" s="59" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="F205" s="64"/>
       <c r="G205" s="65"/>
       <c r="H205" s="65"/>
       <c r="I205" s="65"/>
       <c r="J205" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K205" s="66" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="L205" s="66"/>
       <c r="M205" s="66"/>
@@ -12114,22 +12114,22 @@
         <v>414</v>
       </c>
       <c r="D206" s="51" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="E206" s="59" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="F206" s="64">
         <v>45631</v>
       </c>
       <c r="G206" s="65" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="H206" s="65" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="I206" s="65" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="J206" s="66" t="s">
         <v>120</v>
@@ -12143,19 +12143,19 @@
         <v>120</v>
       </c>
       <c r="O206" s="66" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="P206" s="66" t="s">
         <v>120</v>
       </c>
       <c r="Q206" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="R206" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="S206" s="73" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="T206" s="66"/>
       <c r="U206" s="67"/>
@@ -12175,20 +12175,20 @@
         <v>414</v>
       </c>
       <c r="D207" s="51" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="E207" s="59" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="F207" s="64"/>
       <c r="G207" s="65"/>
       <c r="H207" s="65"/>
       <c r="I207" s="65"/>
       <c r="J207" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K207" s="66" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="L207" s="66"/>
       <c r="M207" s="66"/>
@@ -12216,20 +12216,20 @@
         <v>414</v>
       </c>
       <c r="D208" s="51" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="E208" s="59" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="F208" s="64"/>
       <c r="G208" s="65"/>
       <c r="H208" s="65"/>
       <c r="I208" s="65"/>
       <c r="J208" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K208" s="66" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="L208" s="66"/>
       <c r="M208" s="66"/>
@@ -12257,22 +12257,22 @@
         <v>414</v>
       </c>
       <c r="D209" s="51" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="E209" s="59" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="F209" s="64">
         <v>45631</v>
       </c>
       <c r="G209" s="65" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="H209" s="65" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="I209" s="65" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="J209" s="66" t="s">
         <v>120</v>
@@ -12286,19 +12286,19 @@
         <v>120</v>
       </c>
       <c r="O209" s="66" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="P209" s="66" t="s">
         <v>120</v>
       </c>
       <c r="Q209" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="R209" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="S209" s="73" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="T209" s="66"/>
       <c r="U209" s="67"/>
@@ -12318,22 +12318,22 @@
         <v>414</v>
       </c>
       <c r="D210" s="51" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="E210" s="59" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="F210" s="64">
         <v>45635</v>
       </c>
       <c r="G210" s="65" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="H210" s="65" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="I210" s="65" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="J210" s="66" t="s">
         <v>120</v>
@@ -12347,19 +12347,19 @@
         <v>120</v>
       </c>
       <c r="O210" s="66" t="s">
-        <v>531</v>
+        <v>456</v>
       </c>
       <c r="P210" s="66" t="s">
         <v>120</v>
       </c>
       <c r="Q210" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="R210" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="S210" s="73" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="T210" s="66"/>
       <c r="U210" s="67"/>
@@ -12379,22 +12379,22 @@
         <v>414</v>
       </c>
       <c r="D211" s="51" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="E211" s="59" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="F211" s="64">
         <v>45631</v>
       </c>
       <c r="G211" s="65" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="H211" s="65" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="I211" s="65" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="J211" s="66" t="s">
         <v>120</v>
@@ -12408,19 +12408,19 @@
         <v>120</v>
       </c>
       <c r="O211" s="66" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="P211" s="66" t="s">
         <v>120</v>
       </c>
       <c r="Q211" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="R211" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="S211" s="73" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="T211" s="66"/>
       <c r="U211" s="67"/>
@@ -12440,22 +12440,22 @@
         <v>414</v>
       </c>
       <c r="D212" s="51" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="E212" s="59" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="F212" s="53">
         <v>45631</v>
       </c>
       <c r="G212" s="54" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="H212" s="54" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="I212" s="54" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="J212" s="55" t="s">
         <v>120</v>
@@ -12469,19 +12469,19 @@
         <v>120</v>
       </c>
       <c r="O212" s="55" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="P212" s="55" t="s">
         <v>120</v>
       </c>
       <c r="Q212" s="55" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="R212" s="55" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="S212" s="78" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="T212" s="55"/>
       <c r="U212" s="56"/>
@@ -12501,22 +12501,22 @@
         <v>414</v>
       </c>
       <c r="D213" s="41" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="E213" s="42" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="F213" s="64">
         <v>45631</v>
       </c>
       <c r="G213" s="79" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="H213" s="79" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="I213" s="80" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="J213" s="81" t="s">
         <v>120</v>
@@ -12530,19 +12530,19 @@
         <v>120</v>
       </c>
       <c r="O213" s="73" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="P213" s="81" t="s">
         <v>120</v>
       </c>
       <c r="Q213" s="81" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="R213" s="81" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="S213" s="73" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="T213" s="81"/>
       <c r="U213" s="82"/>
@@ -12562,20 +12562,20 @@
         <v>414</v>
       </c>
       <c r="D214" s="50" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="E214" s="52" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="F214" s="64"/>
       <c r="G214" s="65"/>
       <c r="H214" s="65"/>
       <c r="I214" s="65"/>
       <c r="J214" s="66" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="K214" s="66" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="L214" s="66"/>
       <c r="M214" s="66"/>
@@ -12603,10 +12603,10 @@
         <v>100</v>
       </c>
       <c r="D215" s="50" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="E215" s="52" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="F215" s="53"/>
       <c r="G215" s="54"/>
@@ -12640,10 +12640,10 @@
         <v>100</v>
       </c>
       <c r="D216" s="50" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="E216" s="52" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="F216" s="53"/>
       <c r="G216" s="54"/>
@@ -12677,10 +12677,10 @@
         <v>102</v>
       </c>
       <c r="D217" s="41" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="E217" s="42" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="F217" s="43"/>
       <c r="G217" s="44"/>
@@ -12714,10 +12714,10 @@
         <v>102</v>
       </c>
       <c r="D218" s="50" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="E218" s="52" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="F218" s="53"/>
       <c r="G218" s="54"/>
@@ -12751,22 +12751,22 @@
         <v>414</v>
       </c>
       <c r="D219" s="50" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="E219" s="52" t="s">
-        <v>494</v>
-      </c>
-      <c r="F219" s="53">
-        <v>45653</v>
+        <v>486</v>
+      </c>
+      <c r="F219" s="64">
+        <v>45692</v>
       </c>
       <c r="G219" s="54" t="s">
-        <v>495</v>
+        <v>526</v>
       </c>
       <c r="H219" s="54" t="s">
-        <v>496</v>
+        <v>527</v>
       </c>
       <c r="I219" s="54" t="s">
-        <v>497</v>
+        <v>528</v>
       </c>
       <c r="J219" s="55" t="s">
         <v>120</v>
@@ -16917,8 +16917,8 @@
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -16958,42 +16958,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>500</v>
+        <v>489</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -17023,22 +17023,22 @@
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17046,13 +17046,13 @@
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17060,13 +17060,13 @@
         <v>60</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17074,13 +17074,13 @@
         <v>102</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C4" s="12">
         <v>446.447</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17088,13 +17088,13 @@
         <v>69</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17102,13 +17102,13 @@
         <v>78</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -17116,13 +17116,13 @@
         <v>87</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>508</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>518</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -17130,13 +17130,13 @@
         <v>104</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>520</v>
+        <v>509</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -17144,27 +17144,27 @@
         <v>100</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -17172,13 +17172,13 @@
         <v>414</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>508</v>
+        <v>497</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>528</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18160,7 +18160,7 @@
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>529</v>
+        <v>518</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>120</v>
@@ -18168,10 +18168,10 @@
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19185,26 +19185,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A6B8B41AB45FE4E8B23889C5F604192" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="c6632d705a2655bc4ef003303aa3e89d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="228e3216-9b37-47f7-9d85-6e6726edc181" xmlns:ns3="1e0ec522-3181-4f7c-b363-2ace71f6fee9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc3f6e4344a62cf01cb5a4907fa5259c" ns2:_="" ns3:_="">
     <xsd:import namespace="228e3216-9b37-47f7-9d85-6e6726edc181"/>
@@ -19399,10 +19379,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E288F5C3-DA90-4167-B23D-BE3846B1C7D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
+    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19419,20 +19430,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E288F5C3-DA90-4167-B23D-BE3846B1C7D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
-    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Accreditamento Winsap 3.0 Anatomia Patologica #6
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap 3.0
subject_application_version: 20.17.02
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20250204/Winsap_3.0/20.17.02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20250204-2/Winsap_3.0/20.17.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C52122AD-8EC9-4514-ABFD-29C92C06ADC6}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDDEB774-BBAA-4DB6-AAD0-38626E03D853}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2008,31 +2008,31 @@
     <t>2025-02-04T10:48:18Z</t>
   </si>
   <si>
-    <t>2025-02-04T10:55:44Z</t>
-  </si>
-  <si>
-    <t>440e503517887dcb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.a71a4388c14664fc26e635f3b616a6eab07d795b701d9f97963470a3b5a3c7ff.e0bb7c4853^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-02-04T11:04:41Z</t>
-  </si>
-  <si>
-    <t>c15ec2de72bcc112</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.ad0f64eda4cf289190ce3ee1bbdadbf02a18a5888deb3e86d332b19eb5888a64.bf21883adb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-02-04T11:28:20Z</t>
-  </si>
-  <si>
-    <t>d30936b556cc1dd7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.64cf9f7b3941664ec24b7147a6910f9b066d7399aa26950f34b98bb71ccc1651.867a8914a3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-02-04T17:30:09Z</t>
+  </si>
+  <si>
+    <t>f2f6c2f80496e666</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.118195fb0fc3f94ba208728edb9635e5774534d7f4843698ecf26a33b1ea00c0.9275cc4272^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:29:37Z</t>
+  </si>
+  <si>
+    <t>35d022fb1e640f85</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.fe858af3fa7dd00b83361b327bd5f9d59e51bbec0586c4042eb9302e8cb2ad13.6686b864d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-04T17:27:09</t>
+  </si>
+  <si>
+    <t>9b43d790cb9ab46f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.feff2372252646e6a4c8099249fba6c5bef37c00427f6dc225b85281e2ad992b.223a1842a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4475,10 +4475,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
+      <selection pane="bottomRight" activeCell="I213" sqref="I213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11851,13 +11851,13 @@
         <v>45692</v>
       </c>
       <c r="G200" s="65" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H200" s="65" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I200" s="65" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="J200" s="66" t="s">
         <v>120</v>
@@ -12760,13 +12760,13 @@
         <v>45692</v>
       </c>
       <c r="G219" s="54" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="H219" s="54" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="I219" s="54" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="J219" s="55" t="s">
         <v>120</v>
@@ -19185,6 +19185,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A6B8B41AB45FE4E8B23889C5F604192" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="c6632d705a2655bc4ef003303aa3e89d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="228e3216-9b37-47f7-9d85-6e6726edc181" xmlns:ns3="1e0ec522-3181-4f7c-b363-2ace71f6fee9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc3f6e4344a62cf01cb5a4907fa5259c" ns2:_="" ns3:_="">
     <xsd:import namespace="228e3216-9b37-47f7-9d85-6e6726edc181"/>
@@ -19379,27 +19399,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
+    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E288F5C3-DA90-4167-B23D-BE3846B1C7D1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19416,23 +19435,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
-    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Accreditamento Winsap 3.0 Anatomia Patologica #7
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap 3.0
subject_application_version: 20.17.02
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20250204-2/Winsap_3.0/20.17.02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20250206/Winsap_3.0/20.17.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDDEB774-BBAA-4DB6-AAD0-38626E03D853}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B56EF51-10DC-44C8-842D-7A7B8BE5C782}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -2008,31 +2008,31 @@
     <t>2025-02-04T10:48:18Z</t>
   </si>
   <si>
-    <t>2025-02-04T17:30:09Z</t>
-  </si>
-  <si>
-    <t>f2f6c2f80496e666</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.118195fb0fc3f94ba208728edb9635e5774534d7f4843698ecf26a33b1ea00c0.9275cc4272^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:29:37Z</t>
-  </si>
-  <si>
-    <t>35d022fb1e640f85</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.fe858af3fa7dd00b83361b327bd5f9d59e51bbec0586c4042eb9302e8cb2ad13.6686b864d8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-02-04T17:27:09</t>
-  </si>
-  <si>
-    <t>9b43d790cb9ab46f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.feff2372252646e6a4c8099249fba6c5bef37c00427f6dc225b85281e2ad992b.223a1842a9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-02-06T16:48:53Z</t>
+  </si>
+  <si>
+    <t>e830ad3a071aebf2</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.941af1b6db111908ec363b835cde52814437fa27d5afd66fc1a4f07682c9062d.6e947ae071^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-06T16:48:27Z</t>
+  </si>
+  <si>
+    <t>d87d735fa8235e06</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.dee909c66493a655a5040a7184b97386d611d2f33acbac0ad0fb994869d2d8f6.552740e89d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-06T16:48:04Z</t>
+  </si>
+  <si>
+    <t>3531cde50aa39236</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.39396c15b8652f72f5fd0df541e11850a052390d38a3758ec13e7e5131e71c17.c6e37fe2b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4475,10 +4475,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="E198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B200" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I213" sqref="I213"/>
+      <selection pane="bottomRight" activeCell="F199" sqref="F199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11737,7 +11737,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="198" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="77">
         <v>417</v>
       </c>
@@ -11784,7 +11784,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="199" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="77">
         <v>418</v>
       </c>
@@ -11801,16 +11801,16 @@
         <v>418</v>
       </c>
       <c r="F199" s="64">
-        <v>45692</v>
+        <v>45694</v>
       </c>
       <c r="G199" s="65" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="H199" s="65" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="I199" s="65" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="J199" s="66" t="s">
         <v>120</v>
@@ -11831,7 +11831,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="200" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="77">
         <v>419</v>
       </c>
@@ -11848,16 +11848,16 @@
         <v>420</v>
       </c>
       <c r="F200" s="64">
-        <v>45692</v>
+        <v>45694</v>
       </c>
       <c r="G200" s="65" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="H200" s="65" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="I200" s="65" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="J200" s="66" t="s">
         <v>120</v>
@@ -11878,7 +11878,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="201" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:23" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="77">
         <v>423</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="202" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:23" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="77">
         <v>424</v>
       </c>
@@ -11968,7 +11968,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="203" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:23" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="77">
         <v>425</v>
       </c>
@@ -12021,7 +12021,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="204" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="77">
         <v>426</v>
       </c>
@@ -12062,7 +12062,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="205" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="77">
         <v>432</v>
       </c>
@@ -12103,7 +12103,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="206" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="77">
         <v>433</v>
       </c>
@@ -12164,7 +12164,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="207" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="77">
         <v>434</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="208" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="77">
         <v>435</v>
       </c>
@@ -12246,7 +12246,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="209" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="77">
         <v>437</v>
       </c>
@@ -12307,7 +12307,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="210" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="77">
         <v>438</v>
       </c>
@@ -12368,7 +12368,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="211" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A211" s="77">
         <v>440</v>
       </c>
@@ -12429,7 +12429,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="212" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="77">
         <v>441</v>
       </c>
@@ -12490,7 +12490,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="213" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="85">
         <v>442</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="214" spans="1:23" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="77">
         <v>443</v>
       </c>
@@ -12592,7 +12592,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="215" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:23" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="49">
         <v>444</v>
       </c>
@@ -12629,7 +12629,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="216" spans="1:23" ht="11.1" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:23" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A216" s="49">
         <v>445</v>
       </c>
@@ -12666,7 +12666,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="217" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="60">
         <v>446</v>
       </c>
@@ -12703,7 +12703,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="218" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:23" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="49">
         <v>447</v>
       </c>
@@ -12740,7 +12740,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="219" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:23" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="77">
         <v>460</v>
       </c>
@@ -12757,16 +12757,16 @@
         <v>486</v>
       </c>
       <c r="F219" s="64">
-        <v>45692</v>
+        <v>45694</v>
       </c>
       <c r="G219" s="54" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="H219" s="54" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="I219" s="54" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="J219" s="55" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
Accreditamento Winsap 3.0 Anatomia Patologica #8
commonName auth: S1#111ENGINEERING
subject_application_vendor: Engineering Ingegneria Informatica SpA
subject_application_id: Winsap 3.0
subject_application_version: 20.17.02
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Winsap_3.0/20.17.02/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20250206/Winsap_3.0/20.17.02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit.sharepoint.com/sites/FSE2.0Anatomia/Documenti condivisi/FSE 2.0 Anatomia/SESSIONE_20250212/Winsap_3.0/20.17.02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B56EF51-10DC-44C8-842D-7A7B8BE5C782}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{DE2F4BEF-499F-4820-B7E4-E152FAC7ED29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3039EB6-DF93-4E9F-A3FD-89BDBDC87931}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -2008,15 +2008,6 @@
     <t>2025-02-04T10:48:18Z</t>
   </si>
   <si>
-    <t>2025-02-06T16:48:53Z</t>
-  </si>
-  <si>
-    <t>e830ad3a071aebf2</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150907.941af1b6db111908ec363b835cde52814437fa27d5afd66fc1a4f07682c9062d.6e947ae071^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2025-02-06T16:48:27Z</t>
   </si>
   <si>
@@ -2033,6 +2024,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150907.39396c15b8652f72f5fd0df541e11850a052390d38a3758ec13e7e5131e71c17.c6e37fe2b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e49df5a3b80f7150</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150907.4ae894ec611a9c6427705c5e8fecabde29e8ac431d76c6a7b6e9a78aa8b93a67.c4f0e8c419^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-02-12T11:47:25Z</t>
   </si>
 </sst>
 </file>
@@ -4475,10 +4475,10 @@
   <dimension ref="A1:W779"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B200" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E214" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F199" sqref="F199"/>
+      <selection pane="bottomRight" activeCell="H219" sqref="H219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11804,13 +11804,13 @@
         <v>45694</v>
       </c>
       <c r="G199" s="65" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="H199" s="65" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="I199" s="65" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="J199" s="66" t="s">
         <v>120</v>
@@ -11851,13 +11851,13 @@
         <v>45694</v>
       </c>
       <c r="G200" s="65" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="H200" s="65" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I200" s="65" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="J200" s="66" t="s">
         <v>120</v>
@@ -12757,16 +12757,16 @@
         <v>486</v>
       </c>
       <c r="F219" s="64">
-        <v>45694</v>
+        <v>45700</v>
       </c>
       <c r="G219" s="54" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="H219" s="54" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="I219" s="54" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="J219" s="55" t="s">
         <v>120</v>
@@ -19185,26 +19185,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101009A6B8B41AB45FE4E8B23889C5F604192" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="c6632d705a2655bc4ef003303aa3e89d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="228e3216-9b37-47f7-9d85-6e6726edc181" xmlns:ns3="1e0ec522-3181-4f7c-b363-2ace71f6fee9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc3f6e4344a62cf01cb5a4907fa5259c" ns2:_="" ns3:_="">
     <xsd:import namespace="228e3216-9b37-47f7-9d85-6e6726edc181"/>
@@ -19399,10 +19379,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="1e0ec522-3181-4f7c-b363-2ace71f6fee9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="228e3216-9b37-47f7-9d85-6e6726edc181">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E288F5C3-DA90-4167-B23D-BE3846B1C7D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
+    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19419,20 +19430,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E288F5C3-DA90-4167-B23D-BE3846B1C7D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="228e3216-9b37-47f7-9d85-6e6726edc181"/>
-    <ds:schemaRef ds:uri="1e0ec522-3181-4f7c-b363-2ace71f6fee9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>